<commit_message>
sessão de mecânica finalizada
</commit_message>
<xml_diff>
--- a/documents/troubleshooting.xlsx
+++ b/documents/troubleshooting.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Semeq\Desktop\chatbot_hipotese\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60E26248-3D69-4B0C-B668-16AEE1645E4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABFA6238-6252-4E7B-B623-00D6DB825365}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{FECC2DB1-AD25-4A84-8CFF-001A97E8E6FD}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1802" uniqueCount="609">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2116" uniqueCount="753">
   <si>
     <t>type</t>
   </si>
@@ -1862,13 +1862,445 @@
     <t>Clean and inspect the belt; Replace the belt as required.</t>
   </si>
   <si>
-    <t>ui</t>
-  </si>
-  <si>
     <t>Fan output below SCFM</t>
   </si>
   <si>
     <t>Fan Systems</t>
+  </si>
+  <si>
+    <t>Total resistance on system higher than expected</t>
+  </si>
+  <si>
+    <t>Dampers closed or partially closed</t>
+  </si>
+  <si>
+    <t>Speed too slow</t>
+  </si>
+  <si>
+    <t>check to see whether any dampers have been accidentally closed; Open any dampers that should be open.</t>
+  </si>
+  <si>
+    <t>Check the drive belts for slippage; Adjust the tension if the belts are not damaged; Ensure there is adequate lubrication to bearings; Have the electricians check out the motor.</t>
+  </si>
+  <si>
+    <t>Check whether any other fans are discharging into the same outlet as the fan having problems; This could be a design problem; Inform engineering for an evaluation.</t>
+  </si>
+  <si>
+    <t>Fan output below SCFM (continued)</t>
+  </si>
+  <si>
+    <t>Dampers or variable inlet vanes incorrectly set</t>
+  </si>
+  <si>
+    <t>Poor fan inlet conditions, such as choked filters.</t>
+  </si>
+  <si>
+    <t>Atmospheric air induction through ducting leaks</t>
+  </si>
+  <si>
+    <t>Fan rotation wrong</t>
+  </si>
+  <si>
+    <t>Wheel mounted backward on the shaft</t>
+  </si>
+  <si>
+    <t>Readjust the damper control linkage turnbuckles to the calibrated setpoints.</t>
+  </si>
+  <si>
+    <t>Check the pressure differential across the filters, and clean or replace the dirty filters.</t>
+  </si>
+  <si>
+    <t>Walk ducting system down, and check for leaks; An ultrasonic leak detector is an ideal tool to determine exactly where leaks occur.</t>
+  </si>
+  <si>
+    <t>Ensure that the belt drive is not crossed. Have the electricians check the rotation of the motor.</t>
+  </si>
+  <si>
+    <t>Stop the fan, and have maintenance reverse the wheel.</t>
+  </si>
+  <si>
+    <t>Vibration and noise</t>
+  </si>
+  <si>
+    <t>Unbalance due to dirt buildup on fan blades</t>
+  </si>
+  <si>
+    <t>Poor foundations or warped baseplate</t>
+  </si>
+  <si>
+    <t>Check the foundations for cracks and breakage; Report the findings to engineering for resolution.</t>
+  </si>
+  <si>
+    <t>Perform Vibration analysis to determine the magnitude of the problem, and then balance the fan; Water wash the fan blades to remove the buildup of dirt; If the fan operates in a boiler exhaust system or some other high temperature gaseous system, descale the blades.</t>
+  </si>
+  <si>
+    <t>Vibration and noise (continued)</t>
+  </si>
+  <si>
+    <t>Soft-foot conditions</t>
+  </si>
+  <si>
+    <t>No zero cold-spring of ductwork at the fan connecfion</t>
+  </si>
+  <si>
+    <t>Perform vibration analysis to determine the magnitude of the problem, and then align the fan shafts.</t>
+  </si>
+  <si>
+    <t>Perform a soft-foot check on all the feet of the unit to determine if a soft-foot condition is the problem; Add or remove shims to correct condition.</t>
+  </si>
+  <si>
+    <t>Check for ducting distortion if no expansion or flex joint is fitted; Adjust the hangers as needed.</t>
+  </si>
+  <si>
+    <t>Damaged bearings</t>
+  </si>
+  <si>
+    <t>Belt drive misalignment</t>
+  </si>
+  <si>
+    <t>Bad lubrication</t>
+  </si>
+  <si>
+    <t>Ensure that the sheaves are the same width and are properly aligned with each other.</t>
+  </si>
+  <si>
+    <t>Ensure that the correct lubricant is being used and that the bearings are vented during the lubricant application.</t>
+  </si>
+  <si>
+    <t>Damaged bearings (continued)</t>
+  </si>
+  <si>
+    <t>Bent shalt</t>
+  </si>
+  <si>
+    <t>Ensure that the bearing installation practices are correct.</t>
+  </si>
+  <si>
+    <t>When the fan is off, ensure that the unit is tumed to change the resting point periodically to prevent the shaft from sagging due to its own weight; Check the bearing mounts for undue stress due to bad foundations and misaligned ductwork.</t>
+  </si>
+  <si>
+    <t>Misaligned belt drives</t>
+  </si>
+  <si>
+    <t>Ensure that the belts are sitting in the correct sheaves and are aligned to run true in the V-grooves; Check the lineup of the sidewalls of the sheaves with a straightedge or a stretched string.</t>
+  </si>
+  <si>
+    <t>Worn coupling</t>
+  </si>
+  <si>
+    <t>Resonance effect from another machine(s)</t>
+  </si>
+  <si>
+    <t>Fan rotating in wrong direction</t>
+  </si>
+  <si>
+    <t>Conduct a vibration analysis to determine whether the coupling is worn; The wrong grade of lubricant may have been used and accumulated in one spot, causing an unbalanced condition.</t>
+  </si>
+  <si>
+    <t>Perform an evaluation to determine the extent of resonance and to track down the excitation source(s); To temporarily stop resonance-induced vibration, alter the mass of the unit by placing some weight, such as a bag of sand, on the unit.</t>
+  </si>
+  <si>
+    <t>Have electricians check the motor rotation and correct the rotation as required.</t>
+  </si>
+  <si>
+    <t>Bearing overheating</t>
+  </si>
+  <si>
+    <t>Partial offset restriction on inlet side of fan, causing it to unload</t>
+  </si>
+  <si>
+    <t>Overlubrication of bearing</t>
+  </si>
+  <si>
+    <t>Determine the capacity of the bearing, and follow the manufacturer's recommendations for lubrication.</t>
+  </si>
+  <si>
+    <t>Ensure that no foreign objects are causing a partial blockage on the inlet side of the fan; As fan blades turn past the obstruction, they will be unable to carry the full load and deflect.</t>
+  </si>
+  <si>
+    <t>Unbalance</t>
+  </si>
+  <si>
+    <t>Rotate the shaft, and let it roll until it comes to rest on its own to check for static unbalance; Static unbalance can be corrected by hanging an appropriate weight opposite the resting, 6 o'clock position; Engineers who have the proper instrumentation should do more complex balance correction.</t>
+  </si>
+  <si>
+    <t>When the fan is off, make sure the unit is turned off the resting point periodically to prevent the shaft from sagging due to its owm weight; Check for undue stress on bearing mounts because of bad foundations and misaligned ductwork.</t>
+  </si>
+  <si>
+    <t>Bearings overheating (continued)</t>
+  </si>
+  <si>
+    <t>Over-tensioned belts</t>
+  </si>
+  <si>
+    <t>Abnormal axial thrusting caused by misaligned belts</t>
+  </si>
+  <si>
+    <t>Depress the belts at midspan, and measure the deflection to test the belt tension; The deflection should be equal to 1/64" per inch of span between the centers of the driven and driver units.</t>
+  </si>
+  <si>
+    <t>This can be cause by gross misalignment between the driver and the driven units; It can also be caused when one sheave is wider than the other one; To correct either one, align the belts to the center of the V in each sheave.</t>
+  </si>
+  <si>
+    <t>Sheaves that have eccentric bores due to poor machining practices or cast with boss off-center</t>
+  </si>
+  <si>
+    <t>Plug the bore, and remachine it true; Eccentric bores cause the sheaves to turn off center, causing the belts to tension and detension each revolution; This continual jerking back and forth causes the bearings to take a terrible pounding; Keys and setscrews can have the same effect by drawing a sheave ofllcenter when the force is tightened.</t>
+  </si>
+  <si>
+    <t>Steam Traps</t>
+  </si>
+  <si>
+    <t>Trap blowing live steam</t>
+  </si>
+  <si>
+    <t>No prime, bucket, or traps because Trap not primed when originally installed</t>
+  </si>
+  <si>
+    <t>No prime, bucket, or traps because Trap not primed after cleaned</t>
+  </si>
+  <si>
+    <t>Prime the trap.</t>
+  </si>
+  <si>
+    <t>Prime the cleaned trap.</t>
+  </si>
+  <si>
+    <t>Trap blowing live steam (continued)</t>
+  </si>
+  <si>
+    <t>Bypass valve open or leaking</t>
+  </si>
+  <si>
+    <t>Sudden pressure drop</t>
+  </si>
+  <si>
+    <t>Remove or repair the bypass valve.</t>
+  </si>
+  <si>
+    <t>Install a check valve ahead of the trap.</t>
+  </si>
+  <si>
+    <t>Valve mechanism not closing because Scale or dirt lodged in orifice</t>
+  </si>
+  <si>
+    <t>Worn or defective valve or disc mechanism</t>
+  </si>
+  <si>
+    <t>Ruptured bellows (thermostatic traps)</t>
+  </si>
+  <si>
+    <t>Clean the trap.</t>
+  </si>
+  <si>
+    <t>Repair or replace the defective parts.</t>
+  </si>
+  <si>
+    <t>Replace the bellows.</t>
+  </si>
+  <si>
+    <t>Back pressure too high in a thermodynamic trap because Worn or defective parts</t>
+  </si>
+  <si>
+    <t>Back pressure too high in a thermodynamic trap because Trap stuck open</t>
+  </si>
+  <si>
+    <t>Back pressure too high in a thermodynamic trap because Undersized condensate return line or pig tank</t>
+  </si>
+  <si>
+    <t>Back pressure too high in a thermodynamic trap because Blowing flash steam caused by flash steam forming when the condensate is released to a lower or atmospheric pressure</t>
+  </si>
+  <si>
+    <t>Increase the line or pig tank size.</t>
+  </si>
+  <si>
+    <t>No corrective action is required for this normal condition.</t>
+  </si>
+  <si>
+    <t>Pressure too high because Trap rating too low</t>
+  </si>
+  <si>
+    <t>Pressure too high because Orifice enlarged by normal wear</t>
+  </si>
+  <si>
+    <t>Pressure too high because Pressure-reducing valve set too high or broken</t>
+  </si>
+  <si>
+    <t>Pressure too high because System pressure raised</t>
+  </si>
+  <si>
+    <t>Trap not discharging</t>
+  </si>
+  <si>
+    <t>Install the correct size trap.</t>
+  </si>
+  <si>
+    <t>Replace the worn orifice.</t>
+  </si>
+  <si>
+    <t>Readjust or replace the pressure-reducing valve; The valve may require a new diaphragm.</t>
+  </si>
+  <si>
+    <t>Install the correct pressure change assembly.</t>
+  </si>
+  <si>
+    <t>Trap not discharging (continued)</t>
+  </si>
+  <si>
+    <t>Condensate not reaching the trap because Strainer clogged</t>
+  </si>
+  <si>
+    <t>Condensate not reaching the trap because Obstruction in the line to the trap</t>
+  </si>
+  <si>
+    <t>Condensate not reaching the trap because Bypass valve opening or leaking</t>
+  </si>
+  <si>
+    <t>Blow out the screen with air, or replace it.</t>
+  </si>
+  <si>
+    <t>Condensate not reaching the trap because Steam supply line shut off</t>
+  </si>
+  <si>
+    <t>Condensate not reaching the trap because Trap clogged with foreign matter</t>
+  </si>
+  <si>
+    <t>Condensate not reaching the trap because Trap held closed by a defective mechanism</t>
+  </si>
+  <si>
+    <t>Condensate not reaching the trap because High vacuum in the condensate return line</t>
+  </si>
+  <si>
+    <t>Open the steam supply valve.</t>
+  </si>
+  <si>
+    <t>Clean the strainer, and reinstall it.</t>
+  </si>
+  <si>
+    <t>Repair or replace the defective mechanism.</t>
+  </si>
+  <si>
+    <t>No pressure differential across the trap because Blocked or restricted condensate retum line</t>
+  </si>
+  <si>
+    <t>No pressure differential across the trap because Incorrect pressure change assembly</t>
+  </si>
+  <si>
+    <t>Remove the restriction.</t>
+  </si>
+  <si>
+    <t>Continuous discharge from trap</t>
+  </si>
+  <si>
+    <t>Trap too small and undersized for the capacity being handled</t>
+  </si>
+  <si>
+    <t>Trap pressure rating too high</t>
+  </si>
+  <si>
+    <t>Trap clogged</t>
+  </si>
+  <si>
+    <t>Strainer plugged</t>
+  </si>
+  <si>
+    <t>Bellows overstressed in a themiostatic trap</t>
+  </si>
+  <si>
+    <t>Loss of the prime</t>
+  </si>
+  <si>
+    <t>Failure of valve to seat due to worn valve and seat</t>
+  </si>
+  <si>
+    <t>Install the proper size trap.</t>
+  </si>
+  <si>
+    <t>Clean the trap internals, and reinstall the strainer.</t>
+  </si>
+  <si>
+    <t>Clean the strainer.</t>
+  </si>
+  <si>
+    <t>Install a check valve on the inlet side of the trap.</t>
+  </si>
+  <si>
+    <t>Replace the wom parts.</t>
+  </si>
+  <si>
+    <t>Continuous discharge from the trap (continued)</t>
+  </si>
+  <si>
+    <t>Sluggish or uneven heating</t>
+  </si>
+  <si>
+    <t>Scale and dirt deposits under the valve and in the orifice</t>
+  </si>
+  <si>
+    <t>Worn guide pins and lever</t>
+  </si>
+  <si>
+    <t>Capacity margin in trap for heavy starting loads</t>
+  </si>
+  <si>
+    <t>Insufficient air handling capacity on bucket traps</t>
+  </si>
+  <si>
+    <t>Short circuiting by using group traps</t>
+  </si>
+  <si>
+    <t>Replace the worn parts.</t>
+  </si>
+  <si>
+    <t>Install the proper size larger trap.</t>
+  </si>
+  <si>
+    <t>Use thermic buckets, or increase the vent size.</t>
+  </si>
+  <si>
+    <t>When steam traps are grouped, i.e. multiple traps are run into the same line, there is a possibility of condensate backup due to pressure inconsistencies or obstructions; Systems with many traps feeding into one return line are hard to troubleshoot because it is hard to determine which trap has the problem; Pipe traps individually from vessels.</t>
+  </si>
+  <si>
+    <t>Sluggrsh or uneven heating (continued)</t>
+  </si>
+  <si>
+    <t>Back pressure troubles</t>
+  </si>
+  <si>
+    <t>Inadequate steam supply due to pressure valve change</t>
+  </si>
+  <si>
+    <t>Steam pressure-reducing valve setting off</t>
+  </si>
+  <si>
+    <t>Condensate return line too small</t>
+  </si>
+  <si>
+    <t>Other traps blowing steam into header</t>
+  </si>
+  <si>
+    <t>Pig tank vent line plugged</t>
+  </si>
+  <si>
+    <t>Obstruction in return line</t>
+  </si>
+  <si>
+    <t>Excess vacuum in return line</t>
+  </si>
+  <si>
+    <t>Restore normal steam pressure.</t>
+  </si>
+  <si>
+    <t>Readjust or replace the reducing valve.</t>
+  </si>
+  <si>
+    <t>Install a larger condensate return line.</t>
+  </si>
+  <si>
+    <t>Locate and repair other faulty traps.</t>
+  </si>
+  <si>
+    <t>Clean out pig tank vent line.</t>
   </si>
 </sst>
 </file>
@@ -2241,10 +2673,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20BF1FA3-F49E-46EE-B806-EC0466971FE5}">
-  <dimension ref="A1:J309"/>
+  <dimension ref="A1:J352"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A297" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D283" sqref="D283"/>
+    <sheetView tabSelected="1" topLeftCell="A340" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I345" sqref="I345"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8521,7 +8953,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="273" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A273" s="1">
         <v>76</v>
       </c>
@@ -8544,7 +8976,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="274" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A274" s="1">
         <v>76</v>
       </c>
@@ -8567,7 +8999,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="275" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A275" s="1">
         <v>76</v>
       </c>
@@ -8590,7 +9022,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="276" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A276" s="1">
         <v>76</v>
       </c>
@@ -8613,7 +9045,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="277" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A277" s="1">
         <v>76</v>
       </c>
@@ -8636,7 +9068,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="278" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A278" s="1">
         <v>77</v>
       </c>
@@ -8659,7 +9091,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="279" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A279" s="1">
         <v>77</v>
       </c>
@@ -8682,7 +9114,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="280" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A280" s="1">
         <v>77</v>
       </c>
@@ -8705,7 +9137,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="281" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A281" s="1">
         <v>78</v>
       </c>
@@ -8713,22 +9145,22 @@
         <v>4</v>
       </c>
       <c r="C281" t="s">
+        <v>607</v>
+      </c>
+      <c r="D281" t="s">
+        <v>606</v>
+      </c>
+      <c r="E281" t="s">
         <v>608</v>
       </c>
-      <c r="D281" t="s">
-        <v>607</v>
-      </c>
-      <c r="E281" t="s">
-        <v>7</v>
-      </c>
       <c r="F281" t="s">
-        <v>7</v>
-      </c>
-      <c r="I281" t="s">
-        <v>606</v>
-      </c>
-    </row>
-    <row r="282" spans="1:9" x14ac:dyDescent="0.25">
+        <v>613</v>
+      </c>
+      <c r="G281" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="282" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A282" s="1">
         <v>78</v>
       </c>
@@ -8736,16 +9168,22 @@
         <v>4</v>
       </c>
       <c r="C282" t="s">
-        <v>608</v>
+        <v>607</v>
+      </c>
+      <c r="D282" t="s">
+        <v>606</v>
       </c>
       <c r="E282" t="s">
-        <v>7</v>
+        <v>609</v>
       </c>
       <c r="F282" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="283" spans="1:9" x14ac:dyDescent="0.25">
+        <v>611</v>
+      </c>
+      <c r="G282" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="283" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A283" s="1">
         <v>78</v>
       </c>
@@ -8753,16 +9191,22 @@
         <v>4</v>
       </c>
       <c r="C283" t="s">
-        <v>608</v>
+        <v>607</v>
+      </c>
+      <c r="D283" t="s">
+        <v>606</v>
       </c>
       <c r="E283" t="s">
-        <v>7</v>
+        <v>610</v>
       </c>
       <c r="F283" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="284" spans="1:9" x14ac:dyDescent="0.25">
+        <v>612</v>
+      </c>
+      <c r="G283" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="284" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A284" s="1">
         <v>79</v>
       </c>
@@ -8770,16 +9214,22 @@
         <v>4</v>
       </c>
       <c r="C284" t="s">
-        <v>608</v>
+        <v>607</v>
+      </c>
+      <c r="D284" t="s">
+        <v>614</v>
       </c>
       <c r="E284" t="s">
-        <v>7</v>
+        <v>615</v>
       </c>
       <c r="F284" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="285" spans="1:9" x14ac:dyDescent="0.25">
+        <v>620</v>
+      </c>
+      <c r="G284" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="285" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A285" s="1">
         <v>79</v>
       </c>
@@ -8787,16 +9237,22 @@
         <v>4</v>
       </c>
       <c r="C285" t="s">
-        <v>608</v>
+        <v>607</v>
+      </c>
+      <c r="D285" t="s">
+        <v>614</v>
       </c>
       <c r="E285" t="s">
-        <v>7</v>
+        <v>616</v>
       </c>
       <c r="F285" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="286" spans="1:9" x14ac:dyDescent="0.25">
+        <v>621</v>
+      </c>
+      <c r="G285" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="286" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A286" s="1">
         <v>79</v>
       </c>
@@ -8804,16 +9260,22 @@
         <v>4</v>
       </c>
       <c r="C286" t="s">
-        <v>608</v>
+        <v>607</v>
+      </c>
+      <c r="D286" t="s">
+        <v>614</v>
       </c>
       <c r="E286" t="s">
-        <v>7</v>
+        <v>617</v>
       </c>
       <c r="F286" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="287" spans="1:9" x14ac:dyDescent="0.25">
+        <v>622</v>
+      </c>
+      <c r="G286" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="287" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A287" s="1">
         <v>79</v>
       </c>
@@ -8821,16 +9283,22 @@
         <v>4</v>
       </c>
       <c r="C287" t="s">
-        <v>608</v>
+        <v>607</v>
+      </c>
+      <c r="D287" t="s">
+        <v>614</v>
       </c>
       <c r="E287" t="s">
-        <v>7</v>
+        <v>618</v>
       </c>
       <c r="F287" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="288" spans="1:9" x14ac:dyDescent="0.25">
+        <v>623</v>
+      </c>
+      <c r="G287" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="288" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A288" s="1">
         <v>79</v>
       </c>
@@ -8838,16 +9306,22 @@
         <v>4</v>
       </c>
       <c r="C288" t="s">
-        <v>608</v>
+        <v>607</v>
+      </c>
+      <c r="D288" t="s">
+        <v>614</v>
       </c>
       <c r="E288" t="s">
-        <v>7</v>
+        <v>619</v>
       </c>
       <c r="F288" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="289" spans="1:6" x14ac:dyDescent="0.25">
+        <v>624</v>
+      </c>
+      <c r="G288" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="289" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A289" s="1">
         <v>80</v>
       </c>
@@ -8855,16 +9329,22 @@
         <v>4</v>
       </c>
       <c r="C289" t="s">
-        <v>608</v>
+        <v>607</v>
+      </c>
+      <c r="D289" t="s">
+        <v>625</v>
       </c>
       <c r="E289" t="s">
-        <v>7</v>
+        <v>626</v>
       </c>
       <c r="F289" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="290" spans="1:6" x14ac:dyDescent="0.25">
+        <v>629</v>
+      </c>
+      <c r="G289" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="290" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A290" s="1">
         <v>80</v>
       </c>
@@ -8872,16 +9352,22 @@
         <v>4</v>
       </c>
       <c r="C290" t="s">
-        <v>608</v>
+        <v>607</v>
+      </c>
+      <c r="D290" t="s">
+        <v>625</v>
       </c>
       <c r="E290" t="s">
-        <v>7</v>
+        <v>627</v>
       </c>
       <c r="F290" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="291" spans="1:6" x14ac:dyDescent="0.25">
+        <v>628</v>
+      </c>
+      <c r="G290" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="291" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A291" s="1">
         <v>81</v>
       </c>
@@ -8889,16 +9375,22 @@
         <v>4</v>
       </c>
       <c r="C291" t="s">
-        <v>608</v>
+        <v>607</v>
+      </c>
+      <c r="D291" t="s">
+        <v>630</v>
       </c>
       <c r="E291" t="s">
-        <v>7</v>
+        <v>437</v>
       </c>
       <c r="F291" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="292" spans="1:6" x14ac:dyDescent="0.25">
+        <v>633</v>
+      </c>
+      <c r="G291" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="292" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A292" s="1">
         <v>81</v>
       </c>
@@ -8906,16 +9398,22 @@
         <v>4</v>
       </c>
       <c r="C292" t="s">
-        <v>608</v>
+        <v>607</v>
+      </c>
+      <c r="D292" t="s">
+        <v>630</v>
       </c>
       <c r="E292" t="s">
-        <v>7</v>
+        <v>631</v>
       </c>
       <c r="F292" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="293" spans="1:6" x14ac:dyDescent="0.25">
+        <v>634</v>
+      </c>
+      <c r="G292" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="293" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A293" s="1">
         <v>81</v>
       </c>
@@ -8923,16 +9421,22 @@
         <v>4</v>
       </c>
       <c r="C293" t="s">
-        <v>608</v>
+        <v>607</v>
+      </c>
+      <c r="D293" t="s">
+        <v>630</v>
       </c>
       <c r="E293" t="s">
-        <v>7</v>
+        <v>632</v>
       </c>
       <c r="F293" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="294" spans="1:6" x14ac:dyDescent="0.25">
+        <v>635</v>
+      </c>
+      <c r="G293" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="294" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A294" s="1">
         <v>82</v>
       </c>
@@ -8940,16 +9444,22 @@
         <v>4</v>
       </c>
       <c r="C294" t="s">
-        <v>608</v>
+        <v>607</v>
+      </c>
+      <c r="D294" t="s">
+        <v>636</v>
       </c>
       <c r="E294" t="s">
-        <v>7</v>
+        <v>637</v>
       </c>
       <c r="F294" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="295" spans="1:6" x14ac:dyDescent="0.25">
+        <v>639</v>
+      </c>
+      <c r="G294" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="295" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A295" s="1">
         <v>82</v>
       </c>
@@ -8957,16 +9467,22 @@
         <v>4</v>
       </c>
       <c r="C295" t="s">
-        <v>608</v>
+        <v>607</v>
+      </c>
+      <c r="D295" t="s">
+        <v>636</v>
       </c>
       <c r="E295" t="s">
-        <v>7</v>
+        <v>638</v>
       </c>
       <c r="F295" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="296" spans="1:6" x14ac:dyDescent="0.25">
+        <v>640</v>
+      </c>
+      <c r="G295" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="296" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A296" s="1">
         <v>83</v>
       </c>
@@ -8974,16 +9490,22 @@
         <v>4</v>
       </c>
       <c r="C296" t="s">
-        <v>608</v>
+        <v>607</v>
+      </c>
+      <c r="D296" t="s">
+        <v>641</v>
       </c>
       <c r="E296" t="s">
         <v>7</v>
       </c>
       <c r="F296" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="297" spans="1:6" x14ac:dyDescent="0.25">
+        <v>643</v>
+      </c>
+      <c r="G296" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="297" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A297" s="1">
         <v>83</v>
       </c>
@@ -8991,16 +9513,22 @@
         <v>4</v>
       </c>
       <c r="C297" t="s">
-        <v>608</v>
+        <v>607</v>
+      </c>
+      <c r="D297" t="s">
+        <v>641</v>
       </c>
       <c r="E297" t="s">
-        <v>7</v>
+        <v>642</v>
       </c>
       <c r="F297" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="298" spans="1:6" x14ac:dyDescent="0.25">
+        <v>644</v>
+      </c>
+      <c r="G297" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="298" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A298" s="1">
         <v>84</v>
       </c>
@@ -9008,16 +9536,22 @@
         <v>4</v>
       </c>
       <c r="C298" t="s">
-        <v>608</v>
+        <v>607</v>
+      </c>
+      <c r="D298" t="s">
+        <v>641</v>
       </c>
       <c r="E298" t="s">
-        <v>7</v>
+        <v>645</v>
       </c>
       <c r="F298" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="299" spans="1:6" x14ac:dyDescent="0.25">
+        <v>646</v>
+      </c>
+      <c r="G298" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="299" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A299" s="1">
         <v>85</v>
       </c>
@@ -9025,16 +9559,22 @@
         <v>4</v>
       </c>
       <c r="C299" t="s">
-        <v>608</v>
+        <v>607</v>
+      </c>
+      <c r="D299" t="s">
+        <v>641</v>
       </c>
       <c r="E299" t="s">
-        <v>7</v>
+        <v>647</v>
       </c>
       <c r="F299" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="300" spans="1:6" x14ac:dyDescent="0.25">
+        <v>650</v>
+      </c>
+      <c r="G299" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="300" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A300" s="1">
         <v>85</v>
       </c>
@@ -9042,16 +9582,22 @@
         <v>4</v>
       </c>
       <c r="C300" t="s">
-        <v>608</v>
+        <v>607</v>
+      </c>
+      <c r="D300" t="s">
+        <v>641</v>
       </c>
       <c r="E300" t="s">
-        <v>7</v>
+        <v>648</v>
       </c>
       <c r="F300" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="301" spans="1:6" x14ac:dyDescent="0.25">
+        <v>651</v>
+      </c>
+      <c r="G300" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="301" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A301" s="1">
         <v>85</v>
       </c>
@@ -9059,16 +9605,22 @@
         <v>4</v>
       </c>
       <c r="C301" t="s">
-        <v>608</v>
+        <v>607</v>
+      </c>
+      <c r="D301" t="s">
+        <v>641</v>
       </c>
       <c r="E301" t="s">
-        <v>7</v>
+        <v>649</v>
       </c>
       <c r="F301" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="302" spans="1:6" x14ac:dyDescent="0.25">
+        <v>652</v>
+      </c>
+      <c r="G301" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="302" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A302" s="1">
         <v>86</v>
       </c>
@@ -9076,16 +9628,22 @@
         <v>4</v>
       </c>
       <c r="C302" t="s">
-        <v>608</v>
+        <v>607</v>
+      </c>
+      <c r="D302" t="s">
+        <v>641</v>
       </c>
       <c r="E302" t="s">
-        <v>7</v>
+        <v>654</v>
       </c>
       <c r="F302" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="303" spans="1:6" x14ac:dyDescent="0.25">
+        <v>657</v>
+      </c>
+      <c r="G302" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="303" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A303" s="1">
         <v>86</v>
       </c>
@@ -9093,16 +9651,22 @@
         <v>4</v>
       </c>
       <c r="C303" t="s">
-        <v>608</v>
+        <v>607</v>
+      </c>
+      <c r="D303" t="s">
+        <v>653</v>
       </c>
       <c r="E303" t="s">
-        <v>7</v>
+        <v>655</v>
       </c>
       <c r="F303" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="304" spans="1:6" x14ac:dyDescent="0.25">
+        <v>656</v>
+      </c>
+      <c r="G303" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="304" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A304" s="1">
         <v>86</v>
       </c>
@@ -9110,16 +9674,22 @@
         <v>4</v>
       </c>
       <c r="C304" t="s">
-        <v>608</v>
+        <v>607</v>
+      </c>
+      <c r="D304" t="s">
+        <v>653</v>
       </c>
       <c r="E304" t="s">
-        <v>7</v>
+        <v>437</v>
       </c>
       <c r="F304" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="305" spans="1:6" x14ac:dyDescent="0.25">
+        <v>646</v>
+      </c>
+      <c r="G304" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="305" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A305" s="1">
         <v>87</v>
       </c>
@@ -9127,16 +9697,22 @@
         <v>4</v>
       </c>
       <c r="C305" t="s">
-        <v>608</v>
+        <v>607</v>
+      </c>
+      <c r="D305" t="s">
+        <v>661</v>
       </c>
       <c r="E305" t="s">
-        <v>7</v>
+        <v>658</v>
       </c>
       <c r="F305" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="306" spans="1:6" x14ac:dyDescent="0.25">
+        <v>659</v>
+      </c>
+      <c r="G305" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="306" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A306" s="1">
         <v>87</v>
       </c>
@@ -9144,16 +9720,22 @@
         <v>4</v>
       </c>
       <c r="C306" t="s">
-        <v>608</v>
+        <v>607</v>
+      </c>
+      <c r="D306" t="s">
+        <v>661</v>
       </c>
       <c r="E306" t="s">
-        <v>7</v>
+        <v>64</v>
       </c>
       <c r="F306" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="307" spans="1:6" x14ac:dyDescent="0.25">
+        <v>660</v>
+      </c>
+      <c r="G306" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="307" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A307" s="1">
         <v>88</v>
       </c>
@@ -9161,16 +9743,22 @@
         <v>4</v>
       </c>
       <c r="C307" t="s">
-        <v>608</v>
+        <v>607</v>
+      </c>
+      <c r="D307" t="s">
+        <v>661</v>
       </c>
       <c r="E307" t="s">
-        <v>7</v>
+        <v>662</v>
       </c>
       <c r="F307" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="308" spans="1:6" x14ac:dyDescent="0.25">
+        <v>664</v>
+      </c>
+      <c r="G307" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="308" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A308" s="1">
         <v>88</v>
       </c>
@@ -9178,16 +9766,22 @@
         <v>4</v>
       </c>
       <c r="C308" t="s">
-        <v>608</v>
+        <v>607</v>
+      </c>
+      <c r="D308" t="s">
+        <v>661</v>
       </c>
       <c r="E308" t="s">
-        <v>7</v>
+        <v>663</v>
       </c>
       <c r="F308" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="309" spans="1:6" x14ac:dyDescent="0.25">
+        <v>665</v>
+      </c>
+      <c r="G308" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="309" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A309" s="1">
         <v>89</v>
       </c>
@@ -9195,12 +9789,1007 @@
         <v>4</v>
       </c>
       <c r="C309" t="s">
-        <v>608</v>
+        <v>607</v>
+      </c>
+      <c r="D309" t="s">
+        <v>661</v>
       </c>
       <c r="E309" t="s">
-        <v>7</v>
+        <v>666</v>
       </c>
       <c r="F309" t="s">
+        <v>667</v>
+      </c>
+      <c r="G309" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="310" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A310" s="1">
+        <v>90</v>
+      </c>
+      <c r="B310" t="s">
+        <v>4</v>
+      </c>
+      <c r="C310" t="s">
+        <v>668</v>
+      </c>
+      <c r="D310" t="s">
+        <v>669</v>
+      </c>
+      <c r="E310" t="s">
+        <v>670</v>
+      </c>
+      <c r="F310" t="s">
+        <v>672</v>
+      </c>
+      <c r="G310" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="311" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A311" s="1">
+        <v>90</v>
+      </c>
+      <c r="B311" t="s">
+        <v>4</v>
+      </c>
+      <c r="C311" t="s">
+        <v>668</v>
+      </c>
+      <c r="D311" t="s">
+        <v>669</v>
+      </c>
+      <c r="E311" t="s">
+        <v>671</v>
+      </c>
+      <c r="F311" t="s">
+        <v>673</v>
+      </c>
+      <c r="G311" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="312" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A312" s="1">
+        <v>91</v>
+      </c>
+      <c r="B312" t="s">
+        <v>4</v>
+      </c>
+      <c r="C312" t="s">
+        <v>668</v>
+      </c>
+      <c r="D312" t="s">
+        <v>674</v>
+      </c>
+      <c r="E312" t="s">
+        <v>675</v>
+      </c>
+      <c r="F312" t="s">
+        <v>677</v>
+      </c>
+      <c r="G312" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="313" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A313" s="1">
+        <v>91</v>
+      </c>
+      <c r="B313" t="s">
+        <v>4</v>
+      </c>
+      <c r="C313" t="s">
+        <v>668</v>
+      </c>
+      <c r="D313" t="s">
+        <v>674</v>
+      </c>
+      <c r="E313" t="s">
+        <v>676</v>
+      </c>
+      <c r="F313" t="s">
+        <v>678</v>
+      </c>
+      <c r="G313" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="314" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A314" s="1">
+        <v>92</v>
+      </c>
+      <c r="B314" t="s">
+        <v>4</v>
+      </c>
+      <c r="C314" t="s">
+        <v>668</v>
+      </c>
+      <c r="D314" t="s">
+        <v>674</v>
+      </c>
+      <c r="E314" t="s">
+        <v>679</v>
+      </c>
+      <c r="F314" t="s">
+        <v>682</v>
+      </c>
+      <c r="G314" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="315" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A315" s="1">
+        <v>92</v>
+      </c>
+      <c r="B315" t="s">
+        <v>4</v>
+      </c>
+      <c r="C315" t="s">
+        <v>668</v>
+      </c>
+      <c r="D315" t="s">
+        <v>674</v>
+      </c>
+      <c r="E315" t="s">
+        <v>680</v>
+      </c>
+      <c r="F315" t="s">
+        <v>683</v>
+      </c>
+      <c r="G315" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="316" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A316" s="1">
+        <v>92</v>
+      </c>
+      <c r="B316" t="s">
+        <v>4</v>
+      </c>
+      <c r="C316" t="s">
+        <v>668</v>
+      </c>
+      <c r="D316" t="s">
+        <v>674</v>
+      </c>
+      <c r="E316" t="s">
+        <v>681</v>
+      </c>
+      <c r="F316" t="s">
+        <v>684</v>
+      </c>
+      <c r="G316" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="317" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A317" s="1">
+        <v>93</v>
+      </c>
+      <c r="B317" t="s">
+        <v>4</v>
+      </c>
+      <c r="C317" t="s">
+        <v>668</v>
+      </c>
+      <c r="D317" t="s">
+        <v>674</v>
+      </c>
+      <c r="E317" t="s">
+        <v>685</v>
+      </c>
+      <c r="F317" t="s">
+        <v>683</v>
+      </c>
+      <c r="G317" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="318" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A318" s="1">
+        <v>93</v>
+      </c>
+      <c r="B318" t="s">
+        <v>4</v>
+      </c>
+      <c r="C318" t="s">
+        <v>668</v>
+      </c>
+      <c r="D318" t="s">
+        <v>674</v>
+      </c>
+      <c r="E318" t="s">
+        <v>686</v>
+      </c>
+      <c r="F318" t="s">
+        <v>682</v>
+      </c>
+      <c r="G318" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="319" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A319" s="1">
+        <v>93</v>
+      </c>
+      <c r="B319" t="s">
+        <v>4</v>
+      </c>
+      <c r="C319" t="s">
+        <v>668</v>
+      </c>
+      <c r="D319" t="s">
+        <v>674</v>
+      </c>
+      <c r="E319" t="s">
+        <v>687</v>
+      </c>
+      <c r="F319" t="s">
+        <v>689</v>
+      </c>
+      <c r="G319" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="320" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A320" s="1">
+        <v>93</v>
+      </c>
+      <c r="B320" t="s">
+        <v>4</v>
+      </c>
+      <c r="C320" t="s">
+        <v>668</v>
+      </c>
+      <c r="D320" t="s">
+        <v>674</v>
+      </c>
+      <c r="E320" t="s">
+        <v>688</v>
+      </c>
+      <c r="F320" t="s">
+        <v>690</v>
+      </c>
+      <c r="G320" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="321" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A321" s="1">
+        <v>94</v>
+      </c>
+      <c r="B321" t="s">
+        <v>4</v>
+      </c>
+      <c r="C321" t="s">
+        <v>668</v>
+      </c>
+      <c r="D321" t="s">
+        <v>695</v>
+      </c>
+      <c r="E321" t="s">
+        <v>691</v>
+      </c>
+      <c r="F321" t="s">
+        <v>696</v>
+      </c>
+      <c r="G321" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="322" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A322" s="1">
+        <v>94</v>
+      </c>
+      <c r="B322" t="s">
+        <v>4</v>
+      </c>
+      <c r="C322" t="s">
+        <v>668</v>
+      </c>
+      <c r="D322" t="s">
+        <v>695</v>
+      </c>
+      <c r="E322" t="s">
+        <v>692</v>
+      </c>
+      <c r="F322" t="s">
+        <v>697</v>
+      </c>
+      <c r="G322" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="323" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A323" s="1">
+        <v>94</v>
+      </c>
+      <c r="B323" t="s">
+        <v>4</v>
+      </c>
+      <c r="C323" t="s">
+        <v>668</v>
+      </c>
+      <c r="D323" t="s">
+        <v>695</v>
+      </c>
+      <c r="E323" t="s">
+        <v>693</v>
+      </c>
+      <c r="F323" t="s">
+        <v>698</v>
+      </c>
+      <c r="G323" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="324" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A324" s="1">
+        <v>94</v>
+      </c>
+      <c r="B324" t="s">
+        <v>4</v>
+      </c>
+      <c r="C324" t="s">
+        <v>668</v>
+      </c>
+      <c r="D324" t="s">
+        <v>695</v>
+      </c>
+      <c r="E324" t="s">
+        <v>694</v>
+      </c>
+      <c r="F324" t="s">
+        <v>699</v>
+      </c>
+      <c r="G324" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="325" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A325" s="1">
+        <v>95</v>
+      </c>
+      <c r="B325" t="s">
+        <v>4</v>
+      </c>
+      <c r="C325" t="s">
+        <v>668</v>
+      </c>
+      <c r="D325" t="s">
+        <v>700</v>
+      </c>
+      <c r="E325" t="s">
+        <v>701</v>
+      </c>
+      <c r="F325" t="s">
+        <v>704</v>
+      </c>
+      <c r="G325" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="326" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A326" s="1">
+        <v>95</v>
+      </c>
+      <c r="B326" t="s">
+        <v>4</v>
+      </c>
+      <c r="C326" t="s">
+        <v>668</v>
+      </c>
+      <c r="D326" t="s">
+        <v>700</v>
+      </c>
+      <c r="E326" t="s">
+        <v>702</v>
+      </c>
+      <c r="F326" t="s">
+        <v>433</v>
+      </c>
+      <c r="G326" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="327" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A327" s="1">
+        <v>95</v>
+      </c>
+      <c r="B327" t="s">
+        <v>4</v>
+      </c>
+      <c r="C327" t="s">
+        <v>668</v>
+      </c>
+      <c r="D327" t="s">
+        <v>700</v>
+      </c>
+      <c r="E327" t="s">
+        <v>703</v>
+      </c>
+      <c r="F327" t="s">
+        <v>677</v>
+      </c>
+      <c r="G327" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="328" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A328" s="1">
+        <v>96</v>
+      </c>
+      <c r="B328" t="s">
+        <v>4</v>
+      </c>
+      <c r="C328" t="s">
+        <v>668</v>
+      </c>
+      <c r="D328" t="s">
+        <v>700</v>
+      </c>
+      <c r="E328" t="s">
+        <v>705</v>
+      </c>
+      <c r="F328" t="s">
+        <v>709</v>
+      </c>
+      <c r="G328" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="329" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A329" s="1">
+        <v>96</v>
+      </c>
+      <c r="B329" t="s">
+        <v>4</v>
+      </c>
+      <c r="C329" t="s">
+        <v>668</v>
+      </c>
+      <c r="D329" t="s">
+        <v>700</v>
+      </c>
+      <c r="E329" t="s">
+        <v>706</v>
+      </c>
+      <c r="F329" t="s">
+        <v>710</v>
+      </c>
+      <c r="G329" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="330" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A330" s="1">
+        <v>96</v>
+      </c>
+      <c r="B330" t="s">
+        <v>4</v>
+      </c>
+      <c r="C330" t="s">
+        <v>668</v>
+      </c>
+      <c r="D330" t="s">
+        <v>700</v>
+      </c>
+      <c r="E330" t="s">
+        <v>707</v>
+      </c>
+      <c r="F330" t="s">
+        <v>711</v>
+      </c>
+      <c r="G330" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="331" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A331" s="1">
+        <v>96</v>
+      </c>
+      <c r="B331" t="s">
+        <v>4</v>
+      </c>
+      <c r="C331" t="s">
+        <v>668</v>
+      </c>
+      <c r="D331" t="s">
+        <v>700</v>
+      </c>
+      <c r="E331" t="s">
+        <v>708</v>
+      </c>
+      <c r="F331" t="s">
+        <v>699</v>
+      </c>
+      <c r="G331" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="332" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A332" s="1">
+        <v>97</v>
+      </c>
+      <c r="B332" t="s">
+        <v>4</v>
+      </c>
+      <c r="C332" t="s">
+        <v>668</v>
+      </c>
+      <c r="D332" t="s">
+        <v>700</v>
+      </c>
+      <c r="E332" t="s">
+        <v>712</v>
+      </c>
+      <c r="F332" t="s">
+        <v>714</v>
+      </c>
+      <c r="G332" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="333" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A333" s="1">
+        <v>97</v>
+      </c>
+      <c r="B333" t="s">
+        <v>4</v>
+      </c>
+      <c r="C333" t="s">
+        <v>668</v>
+      </c>
+      <c r="D333" t="s">
+        <v>700</v>
+      </c>
+      <c r="E333" t="s">
+        <v>713</v>
+      </c>
+      <c r="F333" t="s">
+        <v>699</v>
+      </c>
+      <c r="G333" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="334" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A334" s="1">
+        <v>98</v>
+      </c>
+      <c r="B334" t="s">
+        <v>4</v>
+      </c>
+      <c r="C334" t="s">
+        <v>668</v>
+      </c>
+      <c r="D334" t="s">
+        <v>715</v>
+      </c>
+      <c r="E334" t="s">
+        <v>716</v>
+      </c>
+      <c r="F334" t="s">
+        <v>723</v>
+      </c>
+      <c r="G334" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="335" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A335" s="1">
+        <v>98</v>
+      </c>
+      <c r="B335" t="s">
+        <v>4</v>
+      </c>
+      <c r="C335" t="s">
+        <v>668</v>
+      </c>
+      <c r="D335" t="s">
+        <v>715</v>
+      </c>
+      <c r="E335" t="s">
+        <v>717</v>
+      </c>
+      <c r="F335" t="s">
+        <v>699</v>
+      </c>
+      <c r="G335" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="336" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A336" s="1">
+        <v>98</v>
+      </c>
+      <c r="B336" t="s">
+        <v>4</v>
+      </c>
+      <c r="C336" t="s">
+        <v>668</v>
+      </c>
+      <c r="D336" t="s">
+        <v>715</v>
+      </c>
+      <c r="E336" t="s">
+        <v>718</v>
+      </c>
+      <c r="F336" t="s">
+        <v>724</v>
+      </c>
+      <c r="G336" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="337" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A337" s="1">
+        <v>98</v>
+      </c>
+      <c r="B337" t="s">
+        <v>4</v>
+      </c>
+      <c r="C337" t="s">
+        <v>668</v>
+      </c>
+      <c r="D337" t="s">
+        <v>715</v>
+      </c>
+      <c r="E337" t="s">
+        <v>719</v>
+      </c>
+      <c r="F337" t="s">
+        <v>725</v>
+      </c>
+      <c r="G337" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="338" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A338" s="1">
+        <v>98</v>
+      </c>
+      <c r="B338" t="s">
+        <v>4</v>
+      </c>
+      <c r="C338" t="s">
+        <v>668</v>
+      </c>
+      <c r="D338" t="s">
+        <v>715</v>
+      </c>
+      <c r="E338" t="s">
+        <v>720</v>
+      </c>
+      <c r="F338" t="s">
+        <v>684</v>
+      </c>
+      <c r="G338" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="339" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A339" s="1">
+        <v>99</v>
+      </c>
+      <c r="B339" t="s">
+        <v>4</v>
+      </c>
+      <c r="C339" t="s">
+        <v>668</v>
+      </c>
+      <c r="D339" t="s">
+        <v>715</v>
+      </c>
+      <c r="E339" t="s">
+        <v>721</v>
+      </c>
+      <c r="F339" t="s">
+        <v>726</v>
+      </c>
+      <c r="G339" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="340" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A340" s="1">
+        <v>98</v>
+      </c>
+      <c r="B340" t="s">
+        <v>4</v>
+      </c>
+      <c r="C340" t="s">
+        <v>668</v>
+      </c>
+      <c r="D340" t="s">
+        <v>715</v>
+      </c>
+      <c r="E340" t="s">
+        <v>722</v>
+      </c>
+      <c r="F340" t="s">
+        <v>727</v>
+      </c>
+      <c r="G340" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="341" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A341" s="1">
+        <v>99</v>
+      </c>
+      <c r="B341" t="s">
+        <v>4</v>
+      </c>
+      <c r="C341" t="s">
+        <v>668</v>
+      </c>
+      <c r="D341" t="s">
+        <v>728</v>
+      </c>
+      <c r="E341" t="s">
+        <v>730</v>
+      </c>
+      <c r="F341" t="s">
+        <v>682</v>
+      </c>
+      <c r="G341" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="342" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A342" s="1">
+        <v>99</v>
+      </c>
+      <c r="B342" t="s">
+        <v>4</v>
+      </c>
+      <c r="C342" t="s">
+        <v>668</v>
+      </c>
+      <c r="D342" t="s">
+        <v>728</v>
+      </c>
+      <c r="E342" t="s">
+        <v>731</v>
+      </c>
+      <c r="F342" t="s">
+        <v>735</v>
+      </c>
+      <c r="G342" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="343" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A343" s="1">
+        <v>99</v>
+      </c>
+      <c r="B343" t="s">
+        <v>4</v>
+      </c>
+      <c r="C343" t="s">
+        <v>668</v>
+      </c>
+      <c r="D343" t="s">
+        <v>729</v>
+      </c>
+      <c r="E343" t="s">
+        <v>732</v>
+      </c>
+      <c r="F343" t="s">
+        <v>736</v>
+      </c>
+      <c r="G343" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="344" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A344" s="1">
+        <v>99</v>
+      </c>
+      <c r="B344" t="s">
+        <v>4</v>
+      </c>
+      <c r="C344" t="s">
+        <v>668</v>
+      </c>
+      <c r="D344" t="s">
+        <v>729</v>
+      </c>
+      <c r="E344" t="s">
+        <v>733</v>
+      </c>
+      <c r="F344" t="s">
+        <v>737</v>
+      </c>
+      <c r="G344" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="345" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A345" s="1">
+        <v>99</v>
+      </c>
+      <c r="B345" t="s">
+        <v>4</v>
+      </c>
+      <c r="C345" t="s">
+        <v>668</v>
+      </c>
+      <c r="D345" t="s">
+        <v>729</v>
+      </c>
+      <c r="E345" t="s">
+        <v>734</v>
+      </c>
+      <c r="F345" t="s">
+        <v>738</v>
+      </c>
+      <c r="G345" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="346" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A346" s="1">
+        <v>100</v>
+      </c>
+      <c r="B346" t="s">
+        <v>4</v>
+      </c>
+      <c r="C346" t="s">
+        <v>668</v>
+      </c>
+      <c r="D346" t="s">
+        <v>739</v>
+      </c>
+      <c r="E346" t="s">
+        <v>741</v>
+      </c>
+      <c r="F346" t="s">
+        <v>748</v>
+      </c>
+      <c r="G346" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="347" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A347" s="1">
+        <v>100</v>
+      </c>
+      <c r="B347" t="s">
+        <v>4</v>
+      </c>
+      <c r="C347" t="s">
+        <v>668</v>
+      </c>
+      <c r="D347" t="s">
+        <v>739</v>
+      </c>
+      <c r="E347" t="s">
+        <v>742</v>
+      </c>
+      <c r="F347" t="s">
+        <v>749</v>
+      </c>
+      <c r="G347" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="348" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A348" s="1">
+        <v>100</v>
+      </c>
+      <c r="B348" t="s">
+        <v>4</v>
+      </c>
+      <c r="C348" t="s">
+        <v>668</v>
+      </c>
+      <c r="D348" t="s">
+        <v>740</v>
+      </c>
+      <c r="E348" t="s">
+        <v>743</v>
+      </c>
+      <c r="F348" t="s">
+        <v>750</v>
+      </c>
+      <c r="G348" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="349" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A349" s="1">
+        <v>100</v>
+      </c>
+      <c r="B349" t="s">
+        <v>4</v>
+      </c>
+      <c r="C349" t="s">
+        <v>668</v>
+      </c>
+      <c r="D349" t="s">
+        <v>740</v>
+      </c>
+      <c r="E349" t="s">
+        <v>744</v>
+      </c>
+      <c r="F349" t="s">
+        <v>751</v>
+      </c>
+      <c r="G349" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="350" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A350" s="1">
+        <v>100</v>
+      </c>
+      <c r="B350" t="s">
+        <v>4</v>
+      </c>
+      <c r="C350" t="s">
+        <v>668</v>
+      </c>
+      <c r="D350" t="s">
+        <v>740</v>
+      </c>
+      <c r="E350" t="s">
+        <v>745</v>
+      </c>
+      <c r="F350" t="s">
+        <v>752</v>
+      </c>
+      <c r="G350" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="351" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A351" s="1">
+        <v>100</v>
+      </c>
+      <c r="B351" t="s">
+        <v>4</v>
+      </c>
+      <c r="C351" t="s">
+        <v>668</v>
+      </c>
+      <c r="D351" t="s">
+        <v>740</v>
+      </c>
+      <c r="E351" t="s">
+        <v>746</v>
+      </c>
+      <c r="F351" t="s">
+        <v>433</v>
+      </c>
+      <c r="G351" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="352" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A352" s="1">
+        <v>100</v>
+      </c>
+      <c r="B352" t="s">
+        <v>4</v>
+      </c>
+      <c r="C352" t="s">
+        <v>668</v>
+      </c>
+      <c r="D352" t="s">
+        <v>740</v>
+      </c>
+      <c r="E352" t="s">
+        <v>747</v>
+      </c>
+      <c r="F352" t="s">
+        <v>699</v>
+      </c>
+      <c r="G352" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>

<commit_message>
problemas da api resolvidos
</commit_message>
<xml_diff>
--- a/documents/troubleshooting.xlsx
+++ b/documents/troubleshooting.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Semeq\Desktop\chatbot_hipotese\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5639FA1-F8D2-4FF1-B900-01F5B17A0185}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4B71566-646A-45A8-8619-74F226D02A07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-20610" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{FECC2DB1-AD25-4A84-8CFF-001A97E8E6FD}"/>
   </bookViews>
@@ -3378,8 +3378,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -3422,7 +3430,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3434,6 +3442,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3914,10 +3923,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20BF1FA3-F49E-46EE-B806-EC0466971FE5}">
-  <dimension ref="A1:F517"/>
+  <dimension ref="A1:L517"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3929,7 +3938,7 @@
     <col min="5" max="6" width="10.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>147</v>
       </c>
@@ -3949,7 +3958,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -3969,7 +3978,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>1</v>
       </c>
@@ -3989,7 +3998,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>1</v>
       </c>
@@ -4008,8 +4017,9 @@
       <c r="F4" s="3" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="L4" s="5"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>1</v>
       </c>
@@ -4029,7 +4039,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>1</v>
       </c>
@@ -4049,7 +4059,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>2</v>
       </c>
@@ -4069,7 +4079,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>2</v>
       </c>
@@ -4089,7 +4099,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>3</v>
       </c>
@@ -4109,7 +4119,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>2</v>
       </c>
@@ -4129,7 +4139,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>2</v>
       </c>
@@ -4149,7 +4159,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>2</v>
       </c>
@@ -4169,7 +4179,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>3</v>
       </c>
@@ -4189,7 +4199,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>3</v>
       </c>
@@ -4209,7 +4219,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>4</v>
       </c>
@@ -4229,7 +4239,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>4</v>
       </c>

</xml_diff>